<commit_message>
Fix more typos and style
</commit_message>
<xml_diff>
--- a/LATEX/deliverable_1/Budget.xlsx
+++ b/LATEX/deliverable_1/Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmigual/Documents/Projects/TFG/LATEX/Deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmigual/Documents/Projects/TFG/LATEX/deliverable_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -93,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +113,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,9 +149,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -467,342 +474,347 @@
   <dimension ref="C5:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="14" width="10.6640625" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="1" customWidth="1"/>
+    <col min="4" max="14" width="10.6640625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="E5" t="s">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C6" t="s">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>120</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>110</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <f t="shared" ref="G6:G12" si="0">D6-E6-F6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <f>D6*$K$23/$D$13</f>
         <v>3189.7894736842104</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>70</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>26</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <f>L6*1.3</f>
         <v>33.800000000000004</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <f>K6*M6</f>
         <v>2366.0000000000005</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C7" t="s">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>80</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>70</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <f t="shared" ref="H7:H12" si="1">D7*$K$23/$D$13</f>
         <v>2126.5263157894738</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>510</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>18</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="1">
         <f t="shared" ref="M7:M8" si="2">L7*1.3</f>
         <v>23.400000000000002</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <f t="shared" ref="N7:N8" si="3">K7*M7</f>
         <v>11934.000000000002</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C8" t="s">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>40</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>20</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>1063.2631578947369</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>180</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>15</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <f t="shared" si="2"/>
         <v>19.5</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <f t="shared" si="3"/>
         <v>3510</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C9" t="s">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>200</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>15</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>110</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <f t="shared" si="1"/>
         <v>5316.3157894736842</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <f>SUM(K6:K8)</f>
         <v>760</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <f>SUM(N6:N8)</f>
         <v>17810</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C10" t="s">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>80</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>10</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>50</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <f t="shared" si="1"/>
         <v>2126.5263157894738</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C11" t="s">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>80</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>10</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>40</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>2126.5263157894738</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C12" t="s">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>160</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>5</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>110</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>4253.0526315789475</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="C13" t="s">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <f>SUM(D6:D12)</f>
         <v>760</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>70</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>510</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="E14">
+      <c r="H13" s="2">
+        <f>SUM(H6:H12)</f>
+        <v>20202</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
         <f>SUM(E6:E12)</f>
         <v>70</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <f>SUM(F6:F12)</f>
         <v>510</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <f>SUM(G6:G12)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="J16" t="s">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="J16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J17" t="s">
+    <row r="17" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J18" t="s">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="1">
         <f>N9</f>
         <v>17810</v>
       </c>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J19" t="s">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="1">
         <v>1001</v>
       </c>
     </row>
-    <row r="20" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J20" t="s">
+    <row r="20" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="1">
         <v>346</v>
       </c>
     </row>
-    <row r="21" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J21" t="s">
+    <row r="21" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="1">
         <f>SUM(K16:K20)</f>
         <v>19240</v>
       </c>
     </row>
-    <row r="22" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J22" t="s">
+    <row r="22" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="1">
         <f>0.05*K21</f>
         <v>962</v>
       </c>
     </row>
-    <row r="23" spans="10:11" x14ac:dyDescent="0.15">
-      <c r="J23" t="s">
+    <row r="23" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="1">
         <f>K22+K21</f>
         <v>20202</v>
       </c>

</xml_diff>